<commit_message>
update cards : systems, txt, and anki package of the deck
</commit_message>
<xml_diff>
--- a/00.Memory_systems/02.Cartes/Cartes_2_systemes.xlsx
+++ b/00.Memory_systems/02.Cartes/Cartes_2_systemes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AADD85D-B9D3-4250-81A2-A9237BB77298}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA37E75-9504-4BB1-9F48-19EFA9CFECEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cartes" sheetId="13" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="cartes-personnages" sheetId="14" r:id="rId4"/>
     <sheet name="cartes-personnages (2)" sheetId="20" r:id="rId5"/>
     <sheet name="2 systèmes - le + a jour" sheetId="21" r:id="rId6"/>
+    <sheet name="2 systèmes - le + a jour - bis" sheetId="22" r:id="rId7"/>
+    <sheet name="pour export" sheetId="23" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="563">
   <si>
     <t>Papa</t>
   </si>
@@ -1246,6 +1248,474 @@
   </si>
   <si>
     <t>2Pac</t>
+  </si>
+  <si>
+    <t>Dalton | tutu, tatoo</t>
+  </si>
+  <si>
+    <t>Naruto | tonneau, tennis</t>
+  </si>
+  <si>
+    <t>Marsupilami | tam-tam, tomate</t>
+  </si>
+  <si>
+    <t>Roger Rabit | tir, terre, tour</t>
+  </si>
+  <si>
+    <t>Lucky Luke | tuile, taule</t>
+  </si>
+  <si>
+    <t>Schtroumpfs | tâche, toge</t>
+  </si>
+  <si>
+    <t>Kirikou | taxi, tacle</t>
+  </si>
+  <si>
+    <t>Vegeta | taf (fumer), tof (photo)</t>
+  </si>
+  <si>
+    <t>Panthère Rose | tapis, toupis</t>
+  </si>
+  <si>
+    <t>Scratch (écureil age de glace) | tasse, tissu</t>
+  </si>
+  <si>
+    <t>Tintin | tue tête -TV</t>
+  </si>
+  <si>
+    <t>Tiana (La princesse grenouille) | tétine -tatane</t>
+  </si>
+  <si>
+    <t>Tom-Tom et Nana | tréfle, totem</t>
+  </si>
+  <si>
+    <t>E.T | catch, catin</t>
+  </si>
+  <si>
+    <t>Neo | canne, canneton</t>
+  </si>
+  <si>
+    <t>Mask | camion -caméa-méa (san goku)</t>
+  </si>
+  <si>
+    <t>Rocky Balboa | car, karaté</t>
+  </si>
+  <si>
+    <t>Luke Skywalker | cale, calin</t>
+  </si>
+  <si>
+    <t>James Bond | cage -cache</t>
+  </si>
+  <si>
+    <t>Captain America | caca, caco</t>
+  </si>
+  <si>
+    <t>Forrest Gump | café, cave</t>
+  </si>
+  <si>
+    <t>Batman | cape, capote</t>
+  </si>
+  <si>
+    <t>Superman | case, casse (noisette)</t>
+  </si>
+  <si>
+    <t>Tati Danielle | cathéter, cathédrale</t>
+  </si>
+  <si>
+    <t>Ethan Hunt | cadenas, cantine</t>
+  </si>
+  <si>
+    <t>Terminator | carreau (vitre, sol), catamaran</t>
+  </si>
+  <si>
+    <t>Daft Punk | pâtes (lustucru), paté</t>
+  </si>
+  <si>
+    <t>NTM | panier, panneau</t>
+  </si>
+  <si>
+    <t>M | pomme, piment</t>
+  </si>
+  <si>
+    <t>Renaud, RATM | bar, barre</t>
+  </si>
+  <si>
+    <t>Lauryn Hill | pile, pêle</t>
+  </si>
+  <si>
+    <t>Jimi Hendrix | pêche (fruit et poisson), poche</t>
+  </si>
+  <si>
+    <t>Kurt Cobain | pack (de bierre), paquet (cadeau)</t>
+  </si>
+  <si>
+    <t>Freddie Mercury, | bave, baffe</t>
+  </si>
+  <si>
+    <t>2Pac | pipe, papier</t>
+  </si>
+  <si>
+    <t>Céline Dion | passe, passoire</t>
+  </si>
+  <si>
+    <t>Tonton David | patate, patte à tarte</t>
+  </si>
+  <si>
+    <t>Tina Turner | patinette, bottine</t>
+  </si>
+  <si>
+    <t>Tom Jones | pique, bathème</t>
+  </si>
+  <si>
+    <t>Dorothée | cote, couteau</t>
+  </si>
+  <si>
+    <t>Nina | cône (orange et glace)</t>
+  </si>
+  <si>
+    <t>Maman | coma, comète</t>
+  </si>
+  <si>
+    <t>Rom | cors, corde</t>
+  </si>
+  <si>
+    <t>Lolo | col, colle</t>
+  </si>
+  <si>
+    <t>Julien | cochon, cauchemard</t>
+  </si>
+  <si>
+    <t>Xav | coq, coco</t>
+  </si>
+  <si>
+    <t>Flo (cousine) | coffre, coiffe</t>
+  </si>
+  <si>
+    <t>Papa | coppa, copeau</t>
+  </si>
+  <si>
+    <t>Zitoon &amp; Sophie | cosse, coussin</t>
+  </si>
+  <si>
+    <t>Tati (Marie &amp; Michelle) | coton tige</t>
+  </si>
+  <si>
+    <t>Ta Nièce (Anaïs) | cotonneux</t>
+  </si>
+  <si>
+    <t>Ta Mère (Jeannette) | cœur (amour &amp; organe)</t>
+  </si>
+  <si>
+    <t>Tr-A | Dalton</t>
+  </si>
+  <si>
+    <t>Tr-2 | Naruto</t>
+  </si>
+  <si>
+    <t>Tr-3 | Marsupilami</t>
+  </si>
+  <si>
+    <t>Tr-4 | Roger Rabit</t>
+  </si>
+  <si>
+    <t>Tr-5 | Lucky Luke</t>
+  </si>
+  <si>
+    <t>Tr-6 | Schtroumpfs</t>
+  </si>
+  <si>
+    <t>Tr-7 | Kirikou</t>
+  </si>
+  <si>
+    <t>Tr-8 | Vegeta</t>
+  </si>
+  <si>
+    <t>Tr-9 | Panthère Rose</t>
+  </si>
+  <si>
+    <t>Tr-10 | Scratch (écureil age de glace)</t>
+  </si>
+  <si>
+    <t>Tr-V | Tintin</t>
+  </si>
+  <si>
+    <t>Tr-D | Tiana (La princesse grenouille)</t>
+  </si>
+  <si>
+    <t>Tr-R | Tom-Tom et Nana</t>
+  </si>
+  <si>
+    <t>Ca-A | E.T</t>
+  </si>
+  <si>
+    <t>Ca-2 | Neo</t>
+  </si>
+  <si>
+    <t>Ca-3 | Mask</t>
+  </si>
+  <si>
+    <t>Ca-4 | Rocky Balboa</t>
+  </si>
+  <si>
+    <t>Ca-5 | Luke Skywalker</t>
+  </si>
+  <si>
+    <t>Ca-6 | James Bond</t>
+  </si>
+  <si>
+    <t>Ca-7 | Captain America</t>
+  </si>
+  <si>
+    <t>Ca-8 | Forrest Gump</t>
+  </si>
+  <si>
+    <t>Ca-9 | Batman</t>
+  </si>
+  <si>
+    <t>Ca-10 | Superman</t>
+  </si>
+  <si>
+    <t>Ca-V | Tati Danielle</t>
+  </si>
+  <si>
+    <t>Ca-D | Ethan Hunt</t>
+  </si>
+  <si>
+    <t>Ca-R | Terminator</t>
+  </si>
+  <si>
+    <t>Pi-A | Daft Punk</t>
+  </si>
+  <si>
+    <t>Pi-2 | NTM</t>
+  </si>
+  <si>
+    <t>Pi-3 | M</t>
+  </si>
+  <si>
+    <t>Pi-4 | Renaud, RATM</t>
+  </si>
+  <si>
+    <t>Pi-5 | Lauryn Hill</t>
+  </si>
+  <si>
+    <t>Pi-6 | Jimi Hendrix</t>
+  </si>
+  <si>
+    <t>Pi-7 | Kurt Cobain</t>
+  </si>
+  <si>
+    <t>Pi-8 | Freddie Mercury,</t>
+  </si>
+  <si>
+    <t>Pi-9 | 2Pac</t>
+  </si>
+  <si>
+    <t>Pi-10 | Céline Dion</t>
+  </si>
+  <si>
+    <t>Pi-V | Tonton David</t>
+  </si>
+  <si>
+    <t>Pi-D | Tina Turner</t>
+  </si>
+  <si>
+    <t>Pi-R | Tom Jones</t>
+  </si>
+  <si>
+    <t>Co-A | Dorothée</t>
+  </si>
+  <si>
+    <t>Co-2 | Nina</t>
+  </si>
+  <si>
+    <t>Co-3 | Maman</t>
+  </si>
+  <si>
+    <t>Co-4 | Rom</t>
+  </si>
+  <si>
+    <t>Co-5 | Lolo</t>
+  </si>
+  <si>
+    <t>Co-6 | Julien</t>
+  </si>
+  <si>
+    <t>Co-7 | Xav</t>
+  </si>
+  <si>
+    <t>Co-8 | Flo (cousine)</t>
+  </si>
+  <si>
+    <t>Co-9 | Papa</t>
+  </si>
+  <si>
+    <t>Co-10 | Zitoon &amp; Sophie</t>
+  </si>
+  <si>
+    <t>Co-V | Tati (Marie &amp; Michelle)</t>
+  </si>
+  <si>
+    <t>Co-D | Ta Nièce (Anaïs)</t>
+  </si>
+  <si>
+    <t>Co-R | Ta Mère (Jeannette)</t>
+  </si>
+  <si>
+    <t>Tr-A | tutu, tatoo</t>
+  </si>
+  <si>
+    <t>Tr-2 | tonneau, tennis</t>
+  </si>
+  <si>
+    <t>Tr-3 | tam-tam, tomate</t>
+  </si>
+  <si>
+    <t>Tr-4 | tir, terre, tour</t>
+  </si>
+  <si>
+    <t>Tr-5 | tuile, taule</t>
+  </si>
+  <si>
+    <t>Tr-6 | tâche, toge</t>
+  </si>
+  <si>
+    <t>Tr-7 | taxi, tacle</t>
+  </si>
+  <si>
+    <t>Tr-8 | taf (fumer), tof (photo)</t>
+  </si>
+  <si>
+    <t>Tr-9 | tapis, toupis</t>
+  </si>
+  <si>
+    <t>Tr-10 | tasse, tissu</t>
+  </si>
+  <si>
+    <t>Tr-V | tue tête -TV</t>
+  </si>
+  <si>
+    <t>Tr-D | tétine -tatane</t>
+  </si>
+  <si>
+    <t>Tr-R | tréfle, totem</t>
+  </si>
+  <si>
+    <t>Ca-A | catch, catin</t>
+  </si>
+  <si>
+    <t>Ca-2 | canne, canneton</t>
+  </si>
+  <si>
+    <t>Ca-3 | camion -caméa-méa (san goku)</t>
+  </si>
+  <si>
+    <t>Ca-4 | car, karaté</t>
+  </si>
+  <si>
+    <t>Ca-5 | cale, calin</t>
+  </si>
+  <si>
+    <t>Ca-6 | cage -cache</t>
+  </si>
+  <si>
+    <t>Ca-7 | caca, caco</t>
+  </si>
+  <si>
+    <t>Ca-8 | café, cave</t>
+  </si>
+  <si>
+    <t>Ca-9 | cape, capote</t>
+  </si>
+  <si>
+    <t>Ca-10 | case, casse (noisette)</t>
+  </si>
+  <si>
+    <t>Ca-V | cathéter, cathédrale</t>
+  </si>
+  <si>
+    <t>Ca-D | cadenas, cantine</t>
+  </si>
+  <si>
+    <t>Ca-R | carreau (vitre, sol), catamaran</t>
+  </si>
+  <si>
+    <t>Pi-A | pâtes (lustucru), paté</t>
+  </si>
+  <si>
+    <t>Pi-2 | panier, panneau</t>
+  </si>
+  <si>
+    <t>Pi-3 | pomme, piment</t>
+  </si>
+  <si>
+    <t>Pi-4 | bar, barre</t>
+  </si>
+  <si>
+    <t>Pi-5 | pile, pêle</t>
+  </si>
+  <si>
+    <t>Pi-6 | pêche (fruit et poisson), poche</t>
+  </si>
+  <si>
+    <t>Pi-7 | pack (de bierre), paquet (cadeau)</t>
+  </si>
+  <si>
+    <t>Pi-8 | bave, baffe</t>
+  </si>
+  <si>
+    <t>Pi-9 | pipe, papier</t>
+  </si>
+  <si>
+    <t>Pi-10 | passe, passoire</t>
+  </si>
+  <si>
+    <t>Pi-V | patate, patte à tarte</t>
+  </si>
+  <si>
+    <t>Pi-D | patinette, bottine</t>
+  </si>
+  <si>
+    <t>Pi-R | pique, bathème</t>
+  </si>
+  <si>
+    <t>Co-A | cote, couteau</t>
+  </si>
+  <si>
+    <t>Co-2 | cône (orange et glace)</t>
+  </si>
+  <si>
+    <t>Co-3 | coma, comète</t>
+  </si>
+  <si>
+    <t>Co-4 | cors, corde</t>
+  </si>
+  <si>
+    <t>Co-5 | col, colle</t>
+  </si>
+  <si>
+    <t>Co-6 | cochon, cauchemard</t>
+  </si>
+  <si>
+    <t>Co-7 | coq, coco</t>
+  </si>
+  <si>
+    <t>Co-8 | coffre, coiffe</t>
+  </si>
+  <si>
+    <t>Co-9 | coppa, copeau</t>
+  </si>
+  <si>
+    <t>Co-10 | cosse, coussin</t>
+  </si>
+  <si>
+    <t>Co-V | coton tige</t>
+  </si>
+  <si>
+    <t>Co-D | cotonneux</t>
+  </si>
+  <si>
+    <t>Co-R | cœur (amour &amp; organe)</t>
   </si>
 </sst>
 </file>
@@ -5124,13 +5594,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B7F0D5-A584-4D0B-BA55-C77C5267DD21}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5708,4 +6179,4100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885C01C4-98CA-4AC3-9C72-5BD7384DCBC5}">
+  <dimension ref="A1:E156"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="str">
+        <f>B1&amp;" | "&amp;C1</f>
+        <v>Dalton | tutu, tatoo</v>
+      </c>
+      <c r="E1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:E53" si="0">B2&amp;" | "&amp;C2</f>
+        <v>Naruto | tonneau, tennis</v>
+      </c>
+      <c r="E2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Marsupilami | tam-tam, tomate</v>
+      </c>
+      <c r="E3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Roger Rabit | tir, terre, tour</v>
+      </c>
+      <c r="E4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Lucky Luke | tuile, taule</v>
+      </c>
+      <c r="E5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Schtroumpfs | tâche, toge</v>
+      </c>
+      <c r="E6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Kirikou | taxi, tacle</v>
+      </c>
+      <c r="E7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Vegeta | taf (fumer), tof (photo)</v>
+      </c>
+      <c r="E8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" t="s">
+        <v>345</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Panthère Rose | tapis, toupis</v>
+      </c>
+      <c r="E9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Scratch (écureil age de glace) | tasse, tissu</v>
+      </c>
+      <c r="E10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Tintin | tue tête -TV</v>
+      </c>
+      <c r="E11" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Tiana (La princesse grenouille) | tétine -tatane</v>
+      </c>
+      <c r="E12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Tom-Tom et Nana | tréfle, totem</v>
+      </c>
+      <c r="E13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>E.T | catch, catin</v>
+      </c>
+      <c r="E14" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Neo | canne, canneton</v>
+      </c>
+      <c r="E15" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C16" t="s">
+        <v>367</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Mask | camion -caméa-méa (san goku)</v>
+      </c>
+      <c r="E16" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Rocky Balboa | car, karaté</v>
+      </c>
+      <c r="E17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Luke Skywalker | cale, calin</v>
+      </c>
+      <c r="E18" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>371</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>James Bond | cage -cache</v>
+      </c>
+      <c r="E19" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Captain America | caca, caco</v>
+      </c>
+      <c r="E20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Forrest Gump | café, cave</v>
+      </c>
+      <c r="E21" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Batman | cape, capote</v>
+      </c>
+      <c r="E22" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Superman | case, casse (noisette)</v>
+      </c>
+      <c r="E23" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Tati Danielle | cathéter, cathédrale</v>
+      </c>
+      <c r="E24" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B25" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ethan Hunt | cadenas, cantine</v>
+      </c>
+      <c r="E25" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Terminator | carreau (vitre, sol), catamaran</v>
+      </c>
+      <c r="E26" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>Daft Punk | pâtes (lustucru), paté</v>
+      </c>
+      <c r="E27" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>344</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>NTM | panier, panneau</v>
+      </c>
+      <c r="E28" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B29" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" t="s">
+        <v>343</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>M | pomme, piment</v>
+      </c>
+      <c r="E29" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B30" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30" t="s">
+        <v>342</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>Renaud, RATM | bar, barre</v>
+      </c>
+      <c r="E30" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C31" t="s">
+        <v>341</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>Lauryn Hill | pile, pêle</v>
+      </c>
+      <c r="E31" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Jimi Hendrix | pêche (fruit et poisson), poche</v>
+      </c>
+      <c r="E32" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Kurt Cobain | pack (de bierre), paquet (cadeau)</v>
+      </c>
+      <c r="E33" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B34" t="s">
+        <v>255</v>
+      </c>
+      <c r="C34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Freddie Mercury, | bave, baffe</v>
+      </c>
+      <c r="E34" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B35" t="s">
+        <v>406</v>
+      </c>
+      <c r="C35" t="s">
+        <v>330</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>2Pac | pipe, papier</v>
+      </c>
+      <c r="E35" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B36" t="s">
+        <v>257</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>Céline Dion | passe, passoire</v>
+      </c>
+      <c r="E36" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>Tonton David | patate, patte à tarte</v>
+      </c>
+      <c r="E37" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" t="s">
+        <v>340</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>Tina Turner | patinette, bottine</v>
+      </c>
+      <c r="E38" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B39" t="s">
+        <v>339</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Tom Jones | pique, bathème</v>
+      </c>
+      <c r="E39" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>Dorothée | cote, couteau</v>
+      </c>
+      <c r="E40" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Nina | cône (orange et glace)</v>
+      </c>
+      <c r="E41" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>Maman | coma, comète</v>
+      </c>
+      <c r="E42" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>Rom | cors, corde</v>
+      </c>
+      <c r="E43" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44" t="s">
+        <v>405</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>Lolo | col, colle</v>
+      </c>
+      <c r="E44" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="B45" t="s">
+        <v>259</v>
+      </c>
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>Julien | cochon, cauchemard</v>
+      </c>
+      <c r="E45" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="B46" t="s">
+        <v>260</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>Xav | coq, coco</v>
+      </c>
+      <c r="E46" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="B47" t="s">
+        <v>261</v>
+      </c>
+      <c r="C47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Flo (cousine) | coffre, coiffe</v>
+      </c>
+      <c r="E47" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>169</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>Papa | coppa, copeau</v>
+      </c>
+      <c r="E48" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="B49" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>Zitoon &amp; Sophie | cosse, coussin</v>
+      </c>
+      <c r="E49" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B50" t="s">
+        <v>263</v>
+      </c>
+      <c r="C50" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>Tati (Marie &amp; Michelle) | coton tige</v>
+      </c>
+      <c r="E50" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>Ta Nièce (Anaïs) | cotonneux</v>
+      </c>
+      <c r="E51" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>Ta Mère (Jeannette) | cœur (amour &amp; organe)</v>
+      </c>
+      <c r="E52" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>Tr-A | Dalton</v>
+      </c>
+      <c r="E53" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" ref="D54:D117" si="1">B54&amp;" | "&amp;C54</f>
+        <v>Tr-2 | Naruto</v>
+      </c>
+      <c r="E54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C55" t="s">
+        <v>238</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-3 | Marsupilami</v>
+      </c>
+      <c r="E55" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>348</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C56" t="s">
+        <v>239</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-4 | Roger Rabit</v>
+      </c>
+      <c r="E56" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>347</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C57" t="s">
+        <v>240</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-5 | Lucky Luke</v>
+      </c>
+      <c r="E57" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>346</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C58" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-6 | Schtroumpfs</v>
+      </c>
+      <c r="E58" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C59" t="s">
+        <v>337</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-7 | Kirikou</v>
+      </c>
+      <c r="E59" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-8 | Vegeta</v>
+      </c>
+      <c r="E60" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>345</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C61" t="s">
+        <v>242</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-9 | Panthère Rose</v>
+      </c>
+      <c r="E61" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C62" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-10 | Scratch (écureil age de glace)</v>
+      </c>
+      <c r="E62" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>360</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="C63" t="s">
+        <v>244</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-V | Tintin</v>
+      </c>
+      <c r="E63" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>362</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C64" t="s">
+        <v>154</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-D | Tiana (La princesse grenouille)</v>
+      </c>
+      <c r="E64" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C65" t="s">
+        <v>245</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-R | Tom-Tom et Nana</v>
+      </c>
+      <c r="E65" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-A | E.T</v>
+      </c>
+      <c r="E66" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C67" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-2 | Neo</v>
+      </c>
+      <c r="E67" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>367</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C68" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-3 | Mask</v>
+      </c>
+      <c r="E68" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C69" t="s">
+        <v>102</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-4 | Rocky Balboa</v>
+      </c>
+      <c r="E69" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C70" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-5 | Luke Skywalker</v>
+      </c>
+      <c r="E70" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>371</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-6 | James Bond</v>
+      </c>
+      <c r="E71" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="C72" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-7 | Captain America</v>
+      </c>
+      <c r="E72" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C73" t="s">
+        <v>248</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-8 | Forrest Gump</v>
+      </c>
+      <c r="E73" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-9 | Batman</v>
+      </c>
+      <c r="E74" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>160</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-10 | Superman</v>
+      </c>
+      <c r="E75" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>54</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="C76" t="s">
+        <v>249</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-V | Tati Danielle</v>
+      </c>
+      <c r="E76" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="C77" t="s">
+        <v>250</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-D | Ethan Hunt</v>
+      </c>
+      <c r="E77" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca-R | Terminator</v>
+      </c>
+      <c r="E78" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C79" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-A | Daft Punk</v>
+      </c>
+      <c r="E79" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>344</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C80" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-2 | NTM</v>
+      </c>
+      <c r="E80" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C81" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-3 | M</v>
+      </c>
+      <c r="E81" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>342</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C82" t="s">
+        <v>338</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-4 | Renaud, RATM</v>
+      </c>
+      <c r="E82" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>341</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C83" t="s">
+        <v>253</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-5 | Lauryn Hill</v>
+      </c>
+      <c r="E83" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C84" t="s">
+        <v>254</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-6 | Jimi Hendrix</v>
+      </c>
+      <c r="E84" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C85" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-7 | Kurt Cobain</v>
+      </c>
+      <c r="E85" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>162</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C86" t="s">
+        <v>255</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-8 | Freddie Mercury,</v>
+      </c>
+      <c r="E86" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>330</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C87" t="s">
+        <v>406</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-9 | 2Pac</v>
+      </c>
+      <c r="E87" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C88" t="s">
+        <v>257</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-10 | Céline Dion</v>
+      </c>
+      <c r="E88" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>64</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C89" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-V | Tonton David</v>
+      </c>
+      <c r="E89" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>340</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C90" t="s">
+        <v>136</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-D | Tina Turner</v>
+      </c>
+      <c r="E90" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C91" t="s">
+        <v>339</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>Pi-R | Tom Jones</v>
+      </c>
+      <c r="E91" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>163</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-A | Dorothée</v>
+      </c>
+      <c r="E92" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-2 | Nina</v>
+      </c>
+      <c r="E93" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>165</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C94" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-3 | Maman</v>
+      </c>
+      <c r="E94" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>166</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-4 | Rom</v>
+      </c>
+      <c r="E95" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>405</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C96" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-5 | Lolo</v>
+      </c>
+      <c r="E96" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C97" t="s">
+        <v>259</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-6 | Julien</v>
+      </c>
+      <c r="E97" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C98" t="s">
+        <v>260</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-7 | Xav</v>
+      </c>
+      <c r="E98" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C99" t="s">
+        <v>261</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-8 | Flo (cousine)</v>
+      </c>
+      <c r="E99" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>169</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C100" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-9 | Papa</v>
+      </c>
+      <c r="E100" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>170</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C101" t="s">
+        <v>262</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-10 | Zitoon &amp; Sophie</v>
+      </c>
+      <c r="E101" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>171</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C102" t="s">
+        <v>263</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-V | Tati (Marie &amp; Michelle)</v>
+      </c>
+      <c r="E102" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>172</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C103" t="s">
+        <v>130</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-D | Ta Nièce (Anaïs)</v>
+      </c>
+      <c r="E103" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C104" t="s">
+        <v>131</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>Co-R | Ta Mère (Jeannette)</v>
+      </c>
+      <c r="E104" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C105" t="s">
+        <v>173</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-A | tutu, tatoo</v>
+      </c>
+      <c r="E105" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C106" t="s">
+        <v>174</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-2 | tonneau, tennis</v>
+      </c>
+      <c r="E106" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>238</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C107" t="s">
+        <v>175</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-3 | tam-tam, tomate</v>
+      </c>
+      <c r="E107" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>239</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C108" t="s">
+        <v>348</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-4 | tir, terre, tour</v>
+      </c>
+      <c r="E108" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>240</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C109" t="s">
+        <v>347</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-5 | tuile, taule</v>
+      </c>
+      <c r="E109" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C110" t="s">
+        <v>346</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-6 | tâche, toge</v>
+      </c>
+      <c r="E110" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>337</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C111" t="s">
+        <v>179</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-7 | taxi, tacle</v>
+      </c>
+      <c r="E111" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C112" t="s">
+        <v>180</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-8 | taf (fumer), tof (photo)</v>
+      </c>
+      <c r="E112" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>242</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C113" t="s">
+        <v>345</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-9 | tapis, toupis</v>
+      </c>
+      <c r="E113" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>243</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-10 | tasse, tissu</v>
+      </c>
+      <c r="E114" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>244</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="C115" t="s">
+        <v>360</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-V | tue tête -TV</v>
+      </c>
+      <c r="E115" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>154</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C116" t="s">
+        <v>362</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-D | tétine -tatane</v>
+      </c>
+      <c r="E116" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>245</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C117" t="s">
+        <v>184</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="1"/>
+        <v>Tr-R | tréfle, totem</v>
+      </c>
+      <c r="E117" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C118" t="s">
+        <v>49</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" ref="D118:D156" si="2">B118&amp;" | "&amp;C118</f>
+        <v>Ca-A | catch, catin</v>
+      </c>
+      <c r="E118" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C119" t="s">
+        <v>44</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-2 | canne, canneton</v>
+      </c>
+      <c r="E119" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>246</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C120" t="s">
+        <v>367</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-3 | camion -caméa-méa (san goku)</v>
+      </c>
+      <c r="E120" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>102</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C121" t="s">
+        <v>48</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-4 | car, karaté</v>
+      </c>
+      <c r="E121" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>103</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C122" t="s">
+        <v>50</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-5 | cale, calin</v>
+      </c>
+      <c r="E122" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C123" t="s">
+        <v>371</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-6 | cage -cache</v>
+      </c>
+      <c r="E123" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>247</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="C124" t="s">
+        <v>159</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-7 | caca, caco</v>
+      </c>
+      <c r="E124" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C125" t="s">
+        <v>5</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-8 | café, cave</v>
+      </c>
+      <c r="E125" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>9</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C126" t="s">
+        <v>52</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-9 | cape, capote</v>
+      </c>
+      <c r="E126" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C127" t="s">
+        <v>160</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-10 | case, casse (noisette)</v>
+      </c>
+      <c r="E127" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>249</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="C128" t="s">
+        <v>54</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-V | cathéter, cathédrale</v>
+      </c>
+      <c r="E128" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>250</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="C129" t="s">
+        <v>25</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-D | cadenas, cantine</v>
+      </c>
+      <c r="E129" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>13</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C130" t="s">
+        <v>55</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="2"/>
+        <v>Ca-R | carreau (vitre, sol), catamaran</v>
+      </c>
+      <c r="E130" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>16</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C131" t="s">
+        <v>161</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-A | pâtes (lustucru), paté</v>
+      </c>
+      <c r="E131" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>24</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C132" t="s">
+        <v>344</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-2 | panier, panneau</v>
+      </c>
+      <c r="E132" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>251</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C133" t="s">
+        <v>343</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-3 | pomme, piment</v>
+      </c>
+      <c r="E133" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>338</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C134" t="s">
+        <v>342</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-4 | bar, barre</v>
+      </c>
+      <c r="E134" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>253</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C135" t="s">
+        <v>341</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-5 | pile, pêle</v>
+      </c>
+      <c r="E135" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>254</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C136" t="s">
+        <v>57</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-6 | pêche (fruit et poisson), poche</v>
+      </c>
+      <c r="E136" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>134</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C137" t="s">
+        <v>58</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-7 | pack (de bierre), paquet (cadeau)</v>
+      </c>
+      <c r="E137" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>255</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C138" t="s">
+        <v>162</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-8 | bave, baffe</v>
+      </c>
+      <c r="E138" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>406</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C139" t="s">
+        <v>330</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-9 | pipe, papier</v>
+      </c>
+      <c r="E139" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>257</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C140" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-10 | passe, passoire</v>
+      </c>
+      <c r="E140" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C141" t="s">
+        <v>64</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-V | patate, patte à tarte</v>
+      </c>
+      <c r="E141" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>136</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C142" t="s">
+        <v>340</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-D | patinette, bottine</v>
+      </c>
+      <c r="E142" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>339</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C143" t="s">
+        <v>61</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="2"/>
+        <v>Pi-R | pique, bathème</v>
+      </c>
+      <c r="E143" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C144" t="s">
+        <v>163</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-A | cote, couteau</v>
+      </c>
+      <c r="E144" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C145" t="s">
+        <v>164</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-2 | cône (orange et glace)</v>
+      </c>
+      <c r="E145" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C146" t="s">
+        <v>165</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-3 | coma, comète</v>
+      </c>
+      <c r="E146" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C147" t="s">
+        <v>166</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-4 | cors, corde</v>
+      </c>
+      <c r="E147" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>258</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C148" t="s">
+        <v>405</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-5 | col, colle</v>
+      </c>
+      <c r="E148" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>259</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C149" t="s">
+        <v>167</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-6 | cochon, cauchemard</v>
+      </c>
+      <c r="E149" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>260</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C150" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-7 | coq, coco</v>
+      </c>
+      <c r="E150" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>261</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C151" t="s">
+        <v>168</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-8 | coffre, coiffe</v>
+      </c>
+      <c r="E151" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C152" t="s">
+        <v>169</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-9 | coppa, copeau</v>
+      </c>
+      <c r="E152" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C153" t="s">
+        <v>170</v>
+      </c>
+      <c r="D153" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-10 | cosse, coussin</v>
+      </c>
+      <c r="E153" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>263</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C154" t="s">
+        <v>171</v>
+      </c>
+      <c r="D154" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-V | coton tige</v>
+      </c>
+      <c r="E154" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>130</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C155" t="s">
+        <v>172</v>
+      </c>
+      <c r="D155" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-D | cotonneux</v>
+      </c>
+      <c r="E155" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>131</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C156" t="s">
+        <v>35</v>
+      </c>
+      <c r="D156" t="str">
+        <f t="shared" si="2"/>
+        <v>Co-R | cœur (amour &amp; organe)</v>
+      </c>
+      <c r="E156" t="s">
+        <v>562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BC995E-A0E4-4295-A7C2-D87119E6C3C5}">
+  <dimension ref="A1:B156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B11" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B14" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B15" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B16" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B18" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B21" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B22" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B23" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B24" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B25" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="B26" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B27" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B28" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B29" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B30" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B31" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B32" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B34" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B35" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B36" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="B37" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B38" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B39" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B40" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B41" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B42" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B43" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B44" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="B45" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="B46" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="B47" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B48" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="B49" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B50" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B51" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B52" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>348</v>
+      </c>
+      <c r="B56" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>347</v>
+      </c>
+      <c r="B57" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>346</v>
+      </c>
+      <c r="B58" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>345</v>
+      </c>
+      <c r="B61" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>360</v>
+      </c>
+      <c r="B63" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>362</v>
+      </c>
+      <c r="B64" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>367</v>
+      </c>
+      <c r="B68" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>371</v>
+      </c>
+      <c r="B71" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>160</v>
+      </c>
+      <c r="B75" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>54</v>
+      </c>
+      <c r="B76" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>344</v>
+      </c>
+      <c r="B80" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>342</v>
+      </c>
+      <c r="B82" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>341</v>
+      </c>
+      <c r="B83" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>162</v>
+      </c>
+      <c r="B86" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>330</v>
+      </c>
+      <c r="B87" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>64</v>
+      </c>
+      <c r="B89" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>340</v>
+      </c>
+      <c r="B90" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>163</v>
+      </c>
+      <c r="B92" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>165</v>
+      </c>
+      <c r="B94" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>166</v>
+      </c>
+      <c r="B95" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>405</v>
+      </c>
+      <c r="B96" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B97" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>169</v>
+      </c>
+      <c r="B100" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>170</v>
+      </c>
+      <c r="B101" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>171</v>
+      </c>
+      <c r="B102" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>172</v>
+      </c>
+      <c r="B103" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>238</v>
+      </c>
+      <c r="B107" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>239</v>
+      </c>
+      <c r="B108" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>240</v>
+      </c>
+      <c r="B109" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>337</v>
+      </c>
+      <c r="B111" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>242</v>
+      </c>
+      <c r="B113" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>243</v>
+      </c>
+      <c r="B114" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>244</v>
+      </c>
+      <c r="B115" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>154</v>
+      </c>
+      <c r="B116" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>245</v>
+      </c>
+      <c r="B117" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>246</v>
+      </c>
+      <c r="B120" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>102</v>
+      </c>
+      <c r="B121" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>103</v>
+      </c>
+      <c r="B122" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>247</v>
+      </c>
+      <c r="B124" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>9</v>
+      </c>
+      <c r="B126" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>249</v>
+      </c>
+      <c r="B128" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>250</v>
+      </c>
+      <c r="B129" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>13</v>
+      </c>
+      <c r="B130" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>16</v>
+      </c>
+      <c r="B131" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>24</v>
+      </c>
+      <c r="B132" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>251</v>
+      </c>
+      <c r="B133" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>338</v>
+      </c>
+      <c r="B134" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>253</v>
+      </c>
+      <c r="B135" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>254</v>
+      </c>
+      <c r="B136" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>134</v>
+      </c>
+      <c r="B137" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>255</v>
+      </c>
+      <c r="B138" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>406</v>
+      </c>
+      <c r="B139" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>257</v>
+      </c>
+      <c r="B140" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>136</v>
+      </c>
+      <c r="B142" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>339</v>
+      </c>
+      <c r="B143" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>258</v>
+      </c>
+      <c r="B148" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>259</v>
+      </c>
+      <c r="B149" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>260</v>
+      </c>
+      <c r="B150" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>261</v>
+      </c>
+      <c r="B151" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B153" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>263</v>
+      </c>
+      <c r="B154" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>130</v>
+      </c>
+      <c r="B155" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>131</v>
+      </c>
+      <c r="B156" t="s">
+        <v>562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>